<commit_message>
Added a whole bunch of new clases, mostly the controllers for the multiple windows. The Login window, and the Register Window.
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\u-life\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CB585D3-0180-48F2-AD5B-F8E52DF62E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9E73A0-F12A-4163-AA8C-FD40F693DBC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{D01F522C-CD57-4B31-8EB4-CE645565B958}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>R6</t>
+  </si>
+  <si>
+    <t>Leer archivo de texto</t>
+  </si>
+  <si>
+    <t>Permite la lectura de un archivo de texto con la información de los asistentes (espectadores y posibles participantes)</t>
+  </si>
+  <si>
+    <t>Ruta del archivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se lee el archivo de texto con la información correctamente </t>
+  </si>
+  <si>
+    <t>Cargar información</t>
+  </si>
+  <si>
+    <t>Permite cargar la información leída del archivo de texto en un árbol binario</t>
   </si>
 </sst>
 </file>
@@ -420,7 +438,7 @@
   <dimension ref="C3:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,21 +467,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>

</xml_diff>

<commit_message>
se agrego los metodos para serealiar al igual que metodos para crear cuentas
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thetr\Documents\Segundo Semestre\APO II\ECLIPSE\Workspace\u-life\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo\Documents\ProyectoFinal\u-life\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9E73A0-F12A-4163-AA8C-FD40F693DBC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{D01F522C-CD57-4B31-8EB4-CE645565B958}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -81,12 +80,60 @@
   </si>
   <si>
     <t>Permite cargar la información leída del archivo de texto en un árbol binario</t>
+  </si>
+  <si>
+    <t>Crear  nuevas cuentas</t>
+  </si>
+  <si>
+    <t>permite crear nuevas cuentas si el usuario no tiene una</t>
+  </si>
+  <si>
+    <t>datos del usuario</t>
+  </si>
+  <si>
+    <t>nueva cuenta greada</t>
+  </si>
+  <si>
+    <t>Registrar alarmas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le permite al usuario registrar las alarmas que quiera durante el dia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre de la alarma, tiempo que se ejecuta, </t>
+  </si>
+  <si>
+    <t>Alarma guaradada</t>
+  </si>
+  <si>
+    <t>Mostrar alarma</t>
+  </si>
+  <si>
+    <t>Cuando el en el reloj del programa este a la hora de una alarma en especifico se mostrara un anuncio mostrando los datos de la alarma</t>
+  </si>
+  <si>
+    <t>Tiempo que se ejecute la alarma</t>
+  </si>
+  <si>
+    <t>Mensaje mostrando los datos de la alarma</t>
+  </si>
+  <si>
+    <t>Recomendar ejercicios</t>
+  </si>
+  <si>
+    <t>Se debe mostrar al usuario ejercios a diario con los datos del ejercicio</t>
+  </si>
+  <si>
+    <t>Mostrar ejercicio</t>
+  </si>
+  <si>
+    <t>R7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,23 +481,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C654AF1-D328-4FCA-9C02-B2147883C250}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="37.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="7" max="7" width="38.21875" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
@@ -484,7 +531,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -497,99 +544,131 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="60" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>

</xml_diff>

<commit_message>
Aded to the functional requirements
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Leer archivo de texto</t>
   </si>
   <si>
-    <t>Permite la lectura de un archivo de texto con la información de los asistentes (espectadores y posibles participantes)</t>
-  </si>
-  <si>
     <t>Ruta del archivo</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Cargar información</t>
   </si>
   <si>
-    <t>Permite cargar la información leída del archivo de texto en un árbol binario</t>
-  </si>
-  <si>
     <t>Crear  nuevas cuentas</t>
   </si>
   <si>
@@ -118,16 +112,190 @@
     <t>Mensaje mostrando los datos de la alarma</t>
   </si>
   <si>
-    <t>Recomendar ejercicios</t>
-  </si>
-  <si>
-    <t>Se debe mostrar al usuario ejercios a diario con los datos del ejercicio</t>
-  </si>
-  <si>
     <t>Mostrar ejercicio</t>
   </si>
   <si>
     <t>R7</t>
+  </si>
+  <si>
+    <t>Crear y guardar actividades</t>
+  </si>
+  <si>
+    <t>se debe ser capaz de crear ejercicios según las entradas del usuario y mostrarlo</t>
+  </si>
+  <si>
+    <t>tiempo en horas y minutos y calorias queamdaas</t>
+  </si>
+  <si>
+    <t>Craer y guardar actividades</t>
+  </si>
+  <si>
+    <t>Se de ser capaz de crear actividades según las entradas del usuario</t>
+  </si>
+  <si>
+    <t>datos de la actividad</t>
+  </si>
+  <si>
+    <t>mostrar actividad</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>Mostrar tips</t>
+  </si>
+  <si>
+    <t>Se debe ser capz de mostrar tips al usuario</t>
+  </si>
+  <si>
+    <t>Entrada de boton</t>
+  </si>
+  <si>
+    <t>Mostrar tips al usuario</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>Mostrar datos de todos los usuarios</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de atraves de una tabla mostrar los datos de todos los usuarios excepto la contraseña</t>
+  </si>
+  <si>
+    <t>entrada de boton</t>
+  </si>
+  <si>
+    <t>Mostrar datos de los usuarios en tabla de trazabilidad</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>Ordenar los datos de los usuarios</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de ordenar cualquiera de los atributos de los usuarios en la tabla</t>
+  </si>
+  <si>
+    <t>Entrada por boton</t>
+  </si>
+  <si>
+    <t>Datos ordenados según la inidcacion del usuario</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>Permite la lectura de un archivo de texto con la información de los datos curiosos</t>
+  </si>
+  <si>
+    <t>Permite cargar la información leída del archivo de texto en una lista enlazada</t>
+  </si>
+  <si>
+    <t>Serealizar datos de los usuarios</t>
+  </si>
+  <si>
+    <t>se debe ser capaz de serealizar las cuentas de todos los usuarios del programa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serealizar los datos de las cuentas </t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>Cargar los datos de las c uentas</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de cargar los datos de las cuentas cuando se empieza el programa</t>
+  </si>
+  <si>
+    <t>Cargar el programa</t>
+  </si>
+  <si>
+    <t>Cargar los datos de todas las cuentas</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>Buscar una cuenta en especifica</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de buscar una cuenta en especifico según un criterio de busqueda</t>
+  </si>
+  <si>
+    <t>Criterio de busqueda</t>
+  </si>
+  <si>
+    <t>Cuenta del usuario</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>Crrear cuenta premium nueva</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de crear una cuenta premium nueva según los datos del usuario</t>
+  </si>
+  <si>
+    <t>Datos del usuario</t>
+  </si>
+  <si>
+    <t>Cuenta premium nueva</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>Crrear una nueva cuenta normal</t>
+  </si>
+  <si>
+    <t>se debe ser capaz de crear una nueva cuenta normal según los datos del usuario</t>
+  </si>
+  <si>
+    <t>Cuenta nueva</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>Acceder a una cuenta</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de acceder a una cuenta en especifico según el un nombre de usuario y contraseña</t>
+  </si>
+  <si>
+    <t>Contraseña y usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceder a la cuenta </t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>Mostrar un reloj con la hora actual</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de mostrar un reloj con la hora actual que funcioe correctamente</t>
+  </si>
+  <si>
+    <t>Mostrar reloj con la hora actual</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>Mostrar animaciones alrededor del logo Ulife</t>
+  </si>
+  <si>
+    <t>Se debe ser capaz de mostrar el movimiento de figuras alrededor del logo de u-life</t>
+  </si>
+  <si>
+    <t>Mostrara animaciones alrededor del logo U-life</t>
   </si>
 </sst>
 </file>
@@ -482,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G18"/>
+  <dimension ref="C3:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
@@ -522,13 +690,13 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
@@ -536,10 +704,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -549,16 +717,16 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
@@ -566,16 +734,16 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="60" x14ac:dyDescent="0.25">
@@ -583,19 +751,19 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:7" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
@@ -605,75 +773,214 @@
       <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished the trace table
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="119">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -127,9 +127,6 @@
     <t>tiempo en horas y minutos y calorias queamdaas</t>
   </si>
   <si>
-    <t>Craer y guardar actividades</t>
-  </si>
-  <si>
     <t>Se de ser capaz de crear actividades según las entradas del usuario</t>
   </si>
   <si>
@@ -296,6 +293,99 @@
   </si>
   <si>
     <t>Mostrara animaciones alrededor del logo U-life</t>
+  </si>
+  <si>
+    <t>Tabla de Trazabilidad:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requerimiento : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metodos </t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>Load info</t>
+  </si>
+  <si>
+    <t>LoadFacts , LoadInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PremiumAccount </t>
+  </si>
+  <si>
+    <t>DoneRegistration</t>
+  </si>
+  <si>
+    <t>ProAppGUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PremiumAccount, ProAppGUI</t>
+  </si>
+  <si>
+    <t>AddAlarm, AddAlarm</t>
+  </si>
+  <si>
+    <t>Account, ProAPPGUI</t>
+  </si>
+  <si>
+    <t>LoadAlarm</t>
+  </si>
+  <si>
+    <t>Craer y guardar Deporte</t>
+  </si>
+  <si>
+    <t>AddActivity, AddActivity</t>
+  </si>
+  <si>
+    <t>ProAppGUI,Account</t>
+  </si>
+  <si>
+    <t>LoadTips,LoadInfo</t>
+  </si>
+  <si>
+    <t>Ulife</t>
+  </si>
+  <si>
+    <t>sortByName,sortByUsername,sortByAge,SortByHeight,SortByWeight</t>
+  </si>
+  <si>
+    <t>LoadData</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LoadData,initialize</t>
+  </si>
+  <si>
+    <t>Ulife,AccountsGUI</t>
+  </si>
+  <si>
+    <t>SaveData</t>
+  </si>
+  <si>
+    <t>SearchWeight, searchHeight</t>
+  </si>
+  <si>
+    <t>CreatePremiumAccount</t>
+  </si>
+  <si>
+    <t>CreateNewUser</t>
+  </si>
+  <si>
+    <t>Ulife,LoginGUI</t>
+  </si>
+  <si>
+    <t>searchAccount,Login</t>
+  </si>
+  <si>
+    <t>initialize</t>
+  </si>
+  <si>
+    <t>ProAPPGUI</t>
+  </si>
+  <si>
+    <t>shine,shutdownlight,move1,move2,alarmshine,alarmdone</t>
   </si>
 </sst>
 </file>
@@ -331,10 +421,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,336 +749,604 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G21"/>
+  <dimension ref="D3:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="7" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="37.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
+    <col min="8" max="8" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F30" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
+      <c r="F39" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D40" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F40" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D41" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="F41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="F42" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="F43" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D44" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="F44" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="F45" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>88</v>
+      <c r="F46" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished the trace table and the corrections on the test design
</commit_message>
<xml_diff>
--- a/docs/Requerimientos y trazabilidad.xlsx
+++ b/docs/Requerimientos y trazabilidad.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="145">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -307,85 +307,163 @@
     <t>Clase</t>
   </si>
   <si>
-    <t>Load info</t>
-  </si>
-  <si>
-    <t>LoadFacts , LoadInfo</t>
-  </si>
-  <si>
     <t xml:space="preserve">PremiumAccount </t>
   </si>
   <si>
-    <t>DoneRegistration</t>
-  </si>
-  <si>
     <t>ProAppGUI</t>
   </si>
   <si>
-    <t xml:space="preserve"> PremiumAccount, ProAppGUI</t>
-  </si>
-  <si>
-    <t>AddAlarm, AddAlarm</t>
-  </si>
-  <si>
-    <t>Account, ProAPPGUI</t>
-  </si>
-  <si>
-    <t>LoadAlarm</t>
-  </si>
-  <si>
     <t>Craer y guardar Deporte</t>
   </si>
   <si>
-    <t>AddActivity, AddActivity</t>
-  </si>
-  <si>
-    <t>ProAppGUI,Account</t>
-  </si>
-  <si>
-    <t>LoadTips,LoadInfo</t>
-  </si>
-  <si>
     <t>Ulife</t>
   </si>
   <si>
-    <t>sortByName,sortByUsername,sortByAge,SortByHeight,SortByWeight</t>
-  </si>
-  <si>
-    <t>LoadData</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LoadData,initialize</t>
-  </si>
-  <si>
-    <t>Ulife,AccountsGUI</t>
-  </si>
-  <si>
-    <t>SaveData</t>
-  </si>
-  <si>
-    <t>SearchWeight, searchHeight</t>
-  </si>
-  <si>
-    <t>CreatePremiumAccount</t>
-  </si>
-  <si>
-    <t>CreateNewUser</t>
-  </si>
-  <si>
-    <t>Ulife,LoginGUI</t>
-  </si>
-  <si>
-    <t>searchAccount,Login</t>
-  </si>
-  <si>
-    <t>initialize</t>
-  </si>
-  <si>
     <t>ProAPPGUI</t>
   </si>
   <si>
-    <t>shine,shutdownlight,move1,move2,alarmshine,alarmdone</t>
+    <t xml:space="preserve"> ProAppGUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PremiumAccount</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ProAPPGUI</t>
+  </si>
+  <si>
+    <t>ProAppGUI,</t>
+  </si>
+  <si>
+    <t>Ulife,</t>
+  </si>
+  <si>
+    <t>AccountGUI</t>
+  </si>
+  <si>
+    <t>Load info()</t>
+  </si>
+  <si>
+    <t>LoadInfo()</t>
+  </si>
+  <si>
+    <t>,initialize()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LoadData()</t>
+  </si>
+  <si>
+    <t>SortByWeight()</t>
+  </si>
+  <si>
+    <t>SortByHeight()</t>
+  </si>
+  <si>
+    <t>sortByAge()</t>
+  </si>
+  <si>
+    <t>sortByUsername()</t>
+  </si>
+  <si>
+    <t>sortByName()</t>
+  </si>
+  <si>
+    <t>SaveData()</t>
+  </si>
+  <si>
+    <t>LoadData()</t>
+  </si>
+  <si>
+    <t>LoadFacts(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>RegisterGUI</t>
+  </si>
+  <si>
+    <t>DoneRegistration(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>AddAlarm(int hour, int min, String time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AddAlarm(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>LoadAlarm(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>AddActivity(String name, int minutes, int hours)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AddActivity(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>AddActivity(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>AddSport(String name, int minutes, int hours,int calories)</t>
+  </si>
+  <si>
+    <t>LoadTips(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>SortWeight(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>SortHeight(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>sortAge(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>sortUsername(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>sortName(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>searchHeight(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>SearchWeight(ActionEvent e)</t>
+  </si>
+  <si>
+    <t>CreatePremiumAccount(String username, String password, int age, double weight, double height, String gender, String nickName, String name)</t>
+  </si>
+  <si>
+    <t>CreateNewUser(String username, String password, int age, double weight, double height, String gender, String nickName, String name)</t>
+  </si>
+  <si>
+    <t>searchAccount(String username, String password)</t>
+  </si>
+  <si>
+    <t>LoginGUI</t>
+  </si>
+  <si>
+    <t>Login(ActionEvent ev)</t>
+  </si>
+  <si>
+    <t>initialize()</t>
+  </si>
+  <si>
+    <t>shine()</t>
+  </si>
+  <si>
+    <t>move2()</t>
+  </si>
+  <si>
+    <t>move1()</t>
+  </si>
+  <si>
+    <t>shutdownlight()</t>
+  </si>
+  <si>
+    <t>alarmshine()</t>
+  </si>
+  <si>
+    <t>alarmdone()</t>
   </si>
 </sst>
 </file>
@@ -409,7 +487,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -417,23 +495,348 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:H46"/>
+  <dimension ref="D3:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +1287,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>32</v>
@@ -1086,270 +1489,492 @@
         <v>88</v>
       </c>
     </row>
+    <row r="27" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="9" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="4" t="s">
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="13"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D32" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="13"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D36" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="13"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="30" spans="4:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="4" t="s">
+      <c r="F38" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="13"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="D31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="4" t="s">
+    </row>
+    <row r="40" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D41" s="13"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D42" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="23"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="4" t="s">
+    </row>
+    <row r="45" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="26"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" s="19"/>
+    </row>
+    <row r="46" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="26"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" s="19"/>
+    </row>
+    <row r="47" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="26"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" s="19"/>
+    </row>
+    <row r="48" spans="4:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="26"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G48" s="19"/>
+      <c r="H48" s="25"/>
+    </row>
+    <row r="49" spans="4:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="26"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="4:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="26"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G50" s="28"/>
+    </row>
+    <row r="51" spans="4:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="26"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G51" s="28"/>
+    </row>
+    <row r="52" spans="4:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="26"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52" s="28"/>
+    </row>
+    <row r="53" spans="4:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="26"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53" s="29"/>
+    </row>
+    <row r="54" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D54" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D55" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D56" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="4:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="13"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G57" s="17"/>
+    </row>
+    <row r="58" spans="4:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D58" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="4:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D59" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D60" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D61" s="30"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D62" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G62" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33" s="4" t="s">
+    <row r="63" spans="4:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G63" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D40" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D41" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D44" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D45" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="4:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="D46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>117</v>
-      </c>
+    <row r="64" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D64" s="13"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G64" s="17"/>
+    </row>
+    <row r="65" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D65" s="13"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G65" s="17"/>
+    </row>
+    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D66" s="13"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G66" s="17"/>
+    </row>
+    <row r="67" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D67" s="13"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G67" s="17"/>
+    </row>
+    <row r="68" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="14"/>
+      <c r="E68" s="16"/>
+      <c r="F68" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G68" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="D63:D68"/>
+    <mergeCell ref="E63:E68"/>
+    <mergeCell ref="G63:G68"/>
+    <mergeCell ref="G44:G48"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="D44:D53"/>
+    <mergeCell ref="E44:E53"/>
+    <mergeCell ref="G49:G53"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>